<commit_message>
remove issue with SE and PE overlapping SRS accessions
</commit_message>
<xml_diff>
--- a/scrape_pubseqs/vivid_seq_public_NGS.xlsx
+++ b/scrape_pubseqs/vivid_seq_public_NGS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/MountPoints/mountedMeshnick/Projects/VivID_Seq/scrape_pubseqs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Seq/scrape_pubseqs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DFEB268-1881-484F-9CE5-40F66191C322}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9B5A10-5345-684D-8AEF-D280DAC03E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="880" windowWidth="11940" windowHeight="15120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="880" windowWidth="18060" windowHeight="12940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL samples" sheetId="3" r:id="rId1"/>
@@ -4581,7 +4581,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4632,6 +4632,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5040,11 +5047,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="387">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5772,8 +5780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B96" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8695,25 +8703,25 @@
       <c r="A109" t="s">
         <v>1027</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="4" t="s">
         <v>1028</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="4">
         <v>2013</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G109" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H109" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8721,25 +8729,25 @@
       <c r="A110" t="s">
         <v>1029</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="4" t="s">
         <v>1030</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="4">
         <v>2013</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G110" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H110" t="s">
+      <c r="H110" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8747,25 +8755,25 @@
       <c r="A111" t="s">
         <v>1031</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="4" t="s">
         <v>1032</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="4">
         <v>2013</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H111" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8773,25 +8781,25 @@
       <c r="A112" t="s">
         <v>1033</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="4" t="s">
         <v>1034</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="4">
         <v>2013</v>
       </c>
-      <c r="G112" t="s">
+      <c r="G112" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H112" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8799,25 +8807,25 @@
       <c r="A113" t="s">
         <v>1035</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="4" t="s">
         <v>1036</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="4">
         <v>2013</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G113" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H113" t="s">
+      <c r="H113" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8825,25 +8833,25 @@
       <c r="A114" t="s">
         <v>1037</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="4" t="s">
         <v>1038</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="4">
         <v>2013</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G114" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H114" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8851,25 +8859,25 @@
       <c r="A115" t="s">
         <v>1039</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="4" t="s">
         <v>1040</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="4">
         <v>2013</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G115" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H115" t="s">
+      <c r="H115" s="4" t="s">
         <v>555</v>
       </c>
     </row>
@@ -8877,25 +8885,25 @@
       <c r="A116" t="s">
         <v>1041</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="4" t="s">
         <v>1042</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="4" t="s">
         <v>922</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="4" t="s">
         <v>1270</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="4" t="s">
         <v>1283</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="4">
         <v>2013</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G116" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H116" t="s">
+      <c r="H116" s="4" t="s">
         <v>555</v>
       </c>
     </row>

</xml_diff>

<commit_message>
no drc smpls in public
</commit_message>
<xml_diff>
--- a/scrape_pubseqs/vivid_seq_public_NGS.xlsx
+++ b/scrape_pubseqs/vivid_seq_public_NGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Seq/scrape_pubseqs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5126EA9F-7FE1-4247-83C8-4438767018D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99534343-3F47-5B49-9622-3A5A1FA9E1B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13800" yWindow="760" windowWidth="22420" windowHeight="20840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5435" uniqueCount="1582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5420" uniqueCount="1577">
   <si>
     <t>Kudat</t>
   </si>
@@ -4758,28 +4758,13 @@
   </si>
   <si>
     <t>Cleveland Clinic Foundation</t>
-  </si>
-  <si>
-    <t>CD1001</t>
-  </si>
-  <si>
-    <t>CD1002</t>
-  </si>
-  <si>
-    <t>CD1003</t>
-  </si>
-  <si>
-    <t>CD</t>
-  </si>
-  <si>
-    <t>This Study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4855,13 +4840,6 @@
     <font>
       <sz val="12"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5273,7 +5251,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5282,7 +5260,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="387">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -6008,10 +5985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I721"/>
+  <dimension ref="A1:I718"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A694" workbookViewId="0">
-      <selection activeCell="A719" sqref="A719:I721"/>
+      <selection activeCell="D728" sqref="D728"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27092,93 +27069,6 @@
       </c>
       <c r="I718" s="7" t="s">
         <v>1524</v>
-      </c>
-    </row>
-    <row r="719" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A719" s="8" t="s">
-        <v>1577</v>
-      </c>
-      <c r="B719" s="8"/>
-      <c r="C719" s="8" t="s">
-        <v>1580</v>
-      </c>
-      <c r="D719" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E719" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F719" s="8">
-        <v>2013</v>
-      </c>
-      <c r="G719" s="8" t="s">
-        <v>1581</v>
-      </c>
-      <c r="H719" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="I719" s="8" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="720" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A720" s="8" t="s">
-        <v>1578</v>
-      </c>
-      <c r="B720" s="8"/>
-      <c r="C720" s="8" t="s">
-        <v>1580</v>
-      </c>
-      <c r="D720" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E720" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F720" s="8">
-        <v>2013</v>
-      </c>
-      <c r="G720" s="8" t="s">
-        <v>1581</v>
-      </c>
-      <c r="H720" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="I720" s="8" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="721" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A721" s="8" t="s">
-        <v>1579</v>
-      </c>
-      <c r="B721" s="8"/>
-      <c r="C721" s="8" t="s">
-        <v>1580</v>
-      </c>
-      <c r="D721" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E721" s="8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F721" s="8">
-        <v>2013</v>
-      </c>
-      <c r="G721" s="8" t="s">
-        <v>1581</v>
-      </c>
-      <c r="H721" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="I721" s="8" t="s">
-        <v>1522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>